<commit_message>
Updated datasets from Daan allowing 500ms gaps
</commit_message>
<xml_diff>
--- a/processed_data/data_gazepath/data_LLL.xlsx
+++ b/processed_data/data_gazepath/data_LLL.xlsx
@@ -461,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>3071</v>
+        <v>1576</v>
       </c>
       <c r="K2">
-        <v>1517</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>2950</v>
+        <v>503</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>3396</v>
+        <v>917</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -618,17 +618,25 @@
       <c r="E6">
         <v>5</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>congruent</t>
+        </is>
+      </c>
+      <c r="G6">
+        <v>8269</v>
+      </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>3313</v>
+        <v>1706</v>
       </c>
       <c r="K6">
-        <v>1404</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +808,7 @@
         <v>915</v>
       </c>
       <c r="K10">
-        <v>1463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -883,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>3387</v>
+        <v>1882</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -926,10 +934,10 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>3083</v>
+        <v>1744</v>
       </c>
       <c r="K13">
-        <v>1555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1052,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>399</v>
@@ -1256,7 +1264,7 @@
         <v>4513</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1351,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1394,7 +1402,7 @@
         <v>361</v>
       </c>
       <c r="K24">
-        <v>1633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1434,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="J25">
-        <v>2345</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>1426</v>
@@ -1550,17 +1558,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>congruent</t>
+          <t>incongruent</t>
         </is>
       </c>
       <c r="G28">
-        <v>8775</v>
+        <v>6857</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>1277</v>
@@ -1692,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="J31">
-        <v>2081</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <v>605</v>
@@ -1934,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1109</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -2057,7 +2065,7 @@
         <v>5197</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -2192,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="J43">
-        <v>3249</v>
+        <v>681</v>
       </c>
       <c r="K43">
         <v>1066</v>
@@ -2601,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>1163</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2741,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <v>1897</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2801,19 +2809,11 @@
       <c r="E59">
         <v>2</v>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>incongruent</t>
-        </is>
-      </c>
-      <c r="G59">
-        <v>9185</v>
-      </c>
       <c r="H59">
         <v>0</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="J68">
-        <v>1298</v>
+        <v>0</v>
       </c>
       <c r="K68">
         <v>377</v>
@@ -3286,7 +3286,7 @@
         <v>5957</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -3355,19 +3355,11 @@
       <c r="E73">
         <v>4</v>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>incongruent</t>
-        </is>
-      </c>
-      <c r="G73">
-        <v>7583</v>
-      </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -3413,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="J74">
-        <v>3080</v>
+        <v>227</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -3528,7 +3520,7 @@
         <v>5235</v>
       </c>
       <c r="H77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -3580,7 +3572,7 @@
         <v>619</v>
       </c>
       <c r="K78">
-        <v>2483</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3698,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>1699</v>
+        <v>0</v>
       </c>
       <c r="K81">
         <v>411</v>
@@ -3784,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="J83">
-        <v>4294</v>
+        <v>769</v>
       </c>
       <c r="K83">
         <v>273</v>
@@ -3818,7 +3810,7 @@
         </is>
       </c>
       <c r="G84">
-        <v>9949</v>
+        <v>5297</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -3870,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="J85">
-        <v>1621</v>
+        <v>0</v>
       </c>
       <c r="K85">
         <v>2492</v>
@@ -3913,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>3660</v>
+        <v>0</v>
       </c>
       <c r="K86">
         <v>0</v>
@@ -3951,7 +3943,7 @@
         <v>687</v>
       </c>
       <c r="K87">
-        <v>4174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4183,14 +4175,22 @@
       <c r="E93">
         <v>6</v>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>congruent</t>
+        </is>
+      </c>
+      <c r="G93">
+        <v>5423</v>
+      </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93">
         <v>0</v>
       </c>
       <c r="J93">
-        <v>3448</v>
+        <v>0</v>
       </c>
       <c r="K93">
         <v>1666</v>
@@ -4220,17 +4220,17 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>incongruent</t>
+          <t>congruent</t>
         </is>
       </c>
       <c r="G94">
-        <v>7543</v>
+        <v>8717</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J94">
         <v>993</v>
@@ -4276,7 +4276,7 @@
         <v>2</v>
       </c>
       <c r="J95">
-        <v>2006</v>
+        <v>695</v>
       </c>
       <c r="K95">
         <v>1414</v>
@@ -4319,7 +4319,7 @@
         <v>1</v>
       </c>
       <c r="J96">
-        <v>1785</v>
+        <v>0</v>
       </c>
       <c r="K96">
         <v>983</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="K97">
-        <v>3533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -4405,7 +4405,7 @@
         <v>0</v>
       </c>
       <c r="J98">
-        <v>3871</v>
+        <v>447</v>
       </c>
       <c r="K98">
         <v>0</v>
@@ -4448,7 +4448,7 @@
         <v>0</v>
       </c>
       <c r="J99">
-        <v>2660</v>
+        <v>495</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -4725,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>3346</v>
+        <v>2005</v>
       </c>
       <c r="K106">
         <v>0</v>
@@ -4771,7 +4771,7 @@
         <v>1567</v>
       </c>
       <c r="K107">
-        <v>1149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -4931,10 +4931,10 @@
         </is>
       </c>
       <c r="G111">
-        <v>5899</v>
+        <v>6953</v>
       </c>
       <c r="H111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I111">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         <v>4933</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I113">
         <v>1</v>
@@ -5139,7 +5139,7 @@
         <v>0</v>
       </c>
       <c r="J116">
-        <v>6379</v>
+        <v>0</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="J117">
-        <v>2187</v>
+        <v>0</v>
       </c>
       <c r="K117">
         <v>2890</v>
@@ -5263,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="K119">
-        <v>989</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -5384,7 +5384,7 @@
         <v>2775</v>
       </c>
       <c r="K122">
-        <v>628</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -5418,7 +5418,7 @@
         <v>5705</v>
       </c>
       <c r="H123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I123">
         <v>1</v>
@@ -6121,17 +6121,17 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>congruent</t>
+          <t>incongruent</t>
         </is>
       </c>
       <c r="G141">
-        <v>9825</v>
+        <v>8211</v>
       </c>
       <c r="H141">
         <v>1</v>
       </c>
       <c r="I141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J141">
         <v>271</v>
@@ -6177,7 +6177,7 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>1107</v>
+        <v>0</v>
       </c>
       <c r="K142">
         <v>0</v>
@@ -6333,7 +6333,7 @@
         <v>0</v>
       </c>
       <c r="J146">
-        <v>1519</v>
+        <v>0</v>
       </c>
       <c r="K146">
         <v>0</v>
@@ -6497,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="J150">
-        <v>1309</v>
+        <v>0</v>
       </c>
       <c r="K150">
         <v>401</v>
@@ -6609,13 +6609,13 @@
         </is>
       </c>
       <c r="G153">
-        <v>6525</v>
+        <v>9725</v>
       </c>
       <c r="H153">
         <v>0</v>
       </c>
       <c r="I153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J153">
         <v>0</v>
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="J156">
-        <v>1241</v>
+        <v>0</v>
       </c>
       <c r="K156">
         <v>1183</v>
@@ -6790,7 +6790,7 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>1976</v>
+        <v>423</v>
       </c>
       <c r="K157">
         <v>1004</v>
@@ -6833,10 +6833,10 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>1954</v>
+        <v>777</v>
       </c>
       <c r="K158">
-        <v>1834</v>
+        <v>627</v>
       </c>
     </row>
     <row r="159">
@@ -6879,7 +6879,7 @@
         <v>951</v>
       </c>
       <c r="K159">
-        <v>2415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -6965,7 +6965,7 @@
         <v>1525</v>
       </c>
       <c r="K161">
-        <v>1411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -7134,10 +7134,10 @@
         <v>0</v>
       </c>
       <c r="J165">
-        <v>1808</v>
+        <v>613</v>
       </c>
       <c r="K165">
-        <v>1993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -7214,13 +7214,13 @@
         <v>4937</v>
       </c>
       <c r="H167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I167">
         <v>0</v>
       </c>
       <c r="J167">
-        <v>2534</v>
+        <v>0</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -7263,7 +7263,7 @@
         <v>1</v>
       </c>
       <c r="J168">
-        <v>3128</v>
+        <v>211</v>
       </c>
       <c r="K168">
         <v>1171</v>
@@ -7352,7 +7352,7 @@
         <v>0</v>
       </c>
       <c r="K170">
-        <v>1707</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -7395,7 +7395,7 @@
         <v>3092</v>
       </c>
       <c r="K171">
-        <v>1860</v>
+        <v>867</v>
       </c>
     </row>
     <row r="172">
@@ -7653,7 +7653,7 @@
         <v>1313</v>
       </c>
       <c r="K177">
-        <v>3066</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178">
@@ -7696,7 +7696,7 @@
         <v>1216</v>
       </c>
       <c r="K178">
-        <v>1742</v>
+        <v>387</v>
       </c>
     </row>
     <row r="179">
@@ -7951,7 +7951,7 @@
         <v>0</v>
       </c>
       <c r="J184">
-        <v>3039</v>
+        <v>683</v>
       </c>
       <c r="K184">
         <v>0</v>
@@ -7994,7 +7994,7 @@
         <v>0</v>
       </c>
       <c r="J185">
-        <v>1569</v>
+        <v>0</v>
       </c>
       <c r="K185">
         <v>1384</v>
@@ -8022,17 +8022,25 @@
       <c r="E186">
         <v>3</v>
       </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>incongruent</t>
+        </is>
+      </c>
+      <c r="G186">
+        <v>6697</v>
+      </c>
       <c r="H186">
         <v>0</v>
       </c>
       <c r="I186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J186">
         <v>679</v>
       </c>
       <c r="K186">
-        <v>1999</v>
+        <v>601</v>
       </c>
     </row>
     <row r="187">
@@ -8072,10 +8080,10 @@
         <v>1</v>
       </c>
       <c r="J187">
-        <v>1795</v>
+        <v>0</v>
       </c>
       <c r="K187">
-        <v>3132</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="188">
@@ -8153,7 +8161,7 @@
         <v>0</v>
       </c>
       <c r="K189">
-        <v>6293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -8408,7 +8416,7 @@
         <v>1</v>
       </c>
       <c r="J195">
-        <v>1906</v>
+        <v>591</v>
       </c>
       <c r="K195">
         <v>1261</v>
@@ -8451,7 +8459,7 @@
         <v>0</v>
       </c>
       <c r="J196">
-        <v>2721</v>
+        <v>1610</v>
       </c>
       <c r="K196">
         <v>0</v>
@@ -8661,7 +8669,7 @@
         <v>2366</v>
       </c>
       <c r="K201">
-        <v>2805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -8721,10 +8729,10 @@
         <v>2</v>
       </c>
       <c r="I203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J203">
-        <v>1236</v>
+        <v>159</v>
       </c>
       <c r="K203">
         <v>835</v>
@@ -8888,7 +8896,7 @@
         <v>1</v>
       </c>
       <c r="J207">
-        <v>2144</v>
+        <v>0</v>
       </c>
       <c r="K207">
         <v>1292</v>
@@ -8916,16 +8924,8 @@
       <c r="E208">
         <v>1</v>
       </c>
-      <c r="F208" t="inlineStr">
-        <is>
-          <t>congruent</t>
-        </is>
-      </c>
-      <c r="G208">
-        <v>5775</v>
-      </c>
       <c r="H208">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I208">
         <v>0</v>
@@ -8959,19 +8959,11 @@
       <c r="E209">
         <v>2</v>
       </c>
-      <c r="F209" t="inlineStr">
-        <is>
-          <t>incongruent</t>
-        </is>
-      </c>
-      <c r="G209">
-        <v>4929</v>
-      </c>
       <c r="H209">
         <v>0</v>
       </c>
       <c r="I209">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J209">
         <v>0</v>
@@ -9002,8 +8994,16 @@
       <c r="E210">
         <v>3</v>
       </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>congruent</t>
+        </is>
+      </c>
+      <c r="G210">
+        <v>5813</v>
+      </c>
       <c r="H210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I210">
         <v>0</v>
@@ -9090,7 +9090,7 @@
         <v>0</v>
       </c>
       <c r="K212">
-        <v>3021</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -9173,7 +9173,7 @@
         <v>0</v>
       </c>
       <c r="J214">
-        <v>4542</v>
+        <v>1264</v>
       </c>
       <c r="K214">
         <v>0</v>
@@ -9259,7 +9259,7 @@
         <v>0</v>
       </c>
       <c r="J216">
-        <v>2613</v>
+        <v>608</v>
       </c>
       <c r="K216">
         <v>937</v>
@@ -9305,7 +9305,7 @@
         <v>1538</v>
       </c>
       <c r="K217">
-        <v>3488</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="218">
@@ -9348,7 +9348,7 @@
         <v>1709</v>
       </c>
       <c r="K218">
-        <v>3386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -9388,7 +9388,7 @@
         <v>0</v>
       </c>
       <c r="J219">
-        <v>5856</v>
+        <v>0</v>
       </c>
       <c r="K219">
         <v>0</v>
@@ -9465,10 +9465,10 @@
         </is>
       </c>
       <c r="G221">
-        <v>6435</v>
+        <v>9141</v>
       </c>
       <c r="H221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I221">
         <v>0</v>
@@ -9727,7 +9727,7 @@
         <v>2755</v>
       </c>
       <c r="K227">
-        <v>879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -9802,7 +9802,7 @@
         <v>1</v>
       </c>
       <c r="J229">
-        <v>1586</v>
+        <v>483</v>
       </c>
       <c r="K229">
         <v>235</v>
@@ -9845,7 +9845,7 @@
         <v>0</v>
       </c>
       <c r="J230">
-        <v>3226</v>
+        <v>237</v>
       </c>
       <c r="K230">
         <v>0</v>
@@ -9888,10 +9888,10 @@
         <v>1</v>
       </c>
       <c r="J231">
-        <v>1787</v>
+        <v>0</v>
       </c>
       <c r="K231">
-        <v>1649</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232">
@@ -9934,7 +9934,7 @@
         <v>2167</v>
       </c>
       <c r="K232">
-        <v>2472</v>
+        <v>717</v>
       </c>
     </row>
     <row r="233">
@@ -10092,7 +10092,7 @@
         <v>795</v>
       </c>
       <c r="K236">
-        <v>1611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -10132,7 +10132,7 @@
         <v>0</v>
       </c>
       <c r="J237">
-        <v>5422</v>
+        <v>447</v>
       </c>
       <c r="K237">
         <v>0</v>
@@ -10218,10 +10218,10 @@
         <v>1</v>
       </c>
       <c r="J239">
-        <v>2794</v>
+        <v>401</v>
       </c>
       <c r="K239">
-        <v>1375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -10261,7 +10261,7 @@
         <v>0</v>
       </c>
       <c r="J240">
-        <v>2940</v>
+        <v>0</v>
       </c>
       <c r="K240">
         <v>2356</v>
@@ -10334,14 +10334,14 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>incongruent</t>
+          <t>congruent</t>
         </is>
       </c>
       <c r="G242">
-        <v>6311</v>
+        <v>4931</v>
       </c>
       <c r="H242">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I242">
         <v>1</v>
@@ -10350,7 +10350,7 @@
         <v>1912</v>
       </c>
       <c r="K242">
-        <v>1405</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -10562,7 +10562,7 @@
         <v>0</v>
       </c>
       <c r="J247">
-        <v>1177</v>
+        <v>0</v>
       </c>
       <c r="K247">
         <v>0</v>
@@ -10605,7 +10605,7 @@
         <v>0</v>
       </c>
       <c r="J248">
-        <v>1604</v>
+        <v>0</v>
       </c>
       <c r="K248">
         <v>0</v>
@@ -10691,7 +10691,7 @@
         <v>0</v>
       </c>
       <c r="J250">
-        <v>2591</v>
+        <v>511</v>
       </c>
       <c r="K250">
         <v>1782</v>
@@ -10734,7 +10734,7 @@
         <v>0</v>
       </c>
       <c r="J251">
-        <v>4508</v>
+        <v>1105</v>
       </c>
       <c r="K251">
         <v>339</v>
@@ -10777,7 +10777,7 @@
         <v>0</v>
       </c>
       <c r="J252">
-        <v>1826</v>
+        <v>411</v>
       </c>
       <c r="K252">
         <v>477</v>
@@ -10812,10 +10812,10 @@
         <v>0</v>
       </c>
       <c r="J253">
-        <v>1557</v>
+        <v>0</v>
       </c>
       <c r="K253">
-        <v>2919</v>
+        <v>261</v>
       </c>
     </row>
     <row r="254">
@@ -10855,7 +10855,7 @@
         <v>0</v>
       </c>
       <c r="J254">
-        <v>3871</v>
+        <v>0</v>
       </c>
       <c r="K254">
         <v>1103</v>
@@ -10898,10 +10898,10 @@
         <v>1</v>
       </c>
       <c r="J255">
-        <v>2606</v>
+        <v>1159</v>
       </c>
       <c r="K255">
-        <v>3395</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="256">
@@ -11332,8 +11332,16 @@
       <c r="E266">
         <v>1</v>
       </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>congruent</t>
+        </is>
+      </c>
+      <c r="G266">
+        <v>5757</v>
+      </c>
       <c r="H266">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I266">
         <v>0</v>
@@ -11382,7 +11390,7 @@
         <v>0</v>
       </c>
       <c r="J267">
-        <v>1063</v>
+        <v>0</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -11425,7 +11433,7 @@
         <v>0</v>
       </c>
       <c r="J268">
-        <v>1629</v>
+        <v>0</v>
       </c>
       <c r="K268">
         <v>0</v>
@@ -11468,7 +11476,7 @@
         <v>1</v>
       </c>
       <c r="J269">
-        <v>1011</v>
+        <v>0</v>
       </c>
       <c r="K269">
         <v>385</v>
@@ -11511,10 +11519,10 @@
         <v>1</v>
       </c>
       <c r="J270">
-        <v>2175</v>
+        <v>0</v>
       </c>
       <c r="K270">
-        <v>1117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -11597,10 +11605,10 @@
         <v>1</v>
       </c>
       <c r="J272">
-        <v>2368</v>
+        <v>163</v>
       </c>
       <c r="K272">
-        <v>1499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -11643,7 +11651,7 @@
         <v>1071</v>
       </c>
       <c r="K273">
-        <v>1697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274">
@@ -11683,10 +11691,10 @@
         <v>1</v>
       </c>
       <c r="J274">
-        <v>2788</v>
+        <v>779</v>
       </c>
       <c r="K274">
-        <v>2574</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="275">
@@ -11764,7 +11772,7 @@
         <v>1630</v>
       </c>
       <c r="K276">
-        <v>3155</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="277">
@@ -11804,7 +11812,7 @@
         <v>1</v>
       </c>
       <c r="J277">
-        <v>3182</v>
+        <v>1245</v>
       </c>
       <c r="K277">
         <v>1572</v>
@@ -12209,7 +12217,7 @@
         <v>2</v>
       </c>
       <c r="J288">
-        <v>1753</v>
+        <v>0</v>
       </c>
       <c r="K288">
         <v>3216</v>
@@ -12295,7 +12303,7 @@
         <v>0</v>
       </c>
       <c r="J290">
-        <v>3460</v>
+        <v>1361</v>
       </c>
       <c r="K290">
         <v>0</v>
@@ -12626,7 +12634,7 @@
         <v>1289</v>
       </c>
       <c r="K298">
-        <v>1503</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299">
@@ -12666,7 +12674,7 @@
         <v>0</v>
       </c>
       <c r="J299">
-        <v>3255</v>
+        <v>1242</v>
       </c>
       <c r="K299">
         <v>385</v>
@@ -12712,7 +12720,7 @@
         <v>777</v>
       </c>
       <c r="K300">
-        <v>2150</v>
+        <v>965</v>
       </c>
     </row>
     <row r="301">
@@ -13115,7 +13123,7 @@
         <v>0</v>
       </c>
       <c r="J310">
-        <v>2492</v>
+        <v>913</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -13473,7 +13481,7 @@
         <v>0</v>
       </c>
       <c r="K319">
-        <v>1203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320">

</xml_diff>